<commit_message>
Refactor data fetching and add service accessibility map
Moved city, gender SMR, and welfare data fetching logic to dedicated modules under graph/python and updated app.py imports accordingly. Added a new route and backend logic for service accessibility map data, including SQL for facility density. Updated CSV, schema, and data loading to support city area. Refactored frontend layout and JS to support the new map and summary panels.
</commit_message>
<xml_diff>
--- a/database/data_raw/01_County&City_Info.xlsx
+++ b/database/data_raw/01_County&City_Info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>city_name</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>population</t>
+  </si>
+  <si>
+    <t>area</t>
   </si>
   <si>
     <t>region</t>
@@ -190,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -213,6 +216,10 @@
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -228,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -243,6 +250,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,7 +473,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.33"/>
+    <col customWidth="1" min="1" max="3" width="8.33"/>
+    <col customWidth="1" min="5" max="26" width="8.33"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -476,382 +490,451 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4">
         <v>2490000.0</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
+      <c r="D2" s="5">
+        <v>271.79</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4">
         <v>3970000.0</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
+      <c r="D3" s="6">
+        <v>2052.57</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4">
         <v>2270000.0</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
+      <c r="D4" s="6">
+        <v>1220.95</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4">
         <v>2810000.0</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
+      <c r="D5" s="6">
+        <v>2214.9</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="4">
         <v>1886000.0</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
+      <c r="D6" s="6">
+        <v>2191.65</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4">
         <v>2770000.0</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>18</v>
+      <c r="D7" s="6">
+        <v>2951.85</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4">
         <v>370000.0</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>7</v>
+      <c r="D8" s="5">
+        <v>132.76</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="4">
         <v>460000.0</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
+      <c r="D9" s="5">
+        <v>104.15</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="4">
         <v>590000.0</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
+      <c r="D10" s="6">
+        <v>1427.59</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="4">
         <v>540000.0</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>15</v>
+      <c r="D11" s="6">
+        <v>1820.31</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4">
         <v>1260000.0</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>15</v>
+      <c r="D12" s="6">
+        <v>1074.39</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" s="4">
         <v>480000.0</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>15</v>
+      <c r="D13" s="6">
+        <v>4106.43</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="4">
         <v>660000.0</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>15</v>
+      <c r="D14" s="6">
+        <v>1290.84</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="4">
         <v>264000.0</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>18</v>
+      <c r="D15" s="5">
+        <v>60.03</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="4">
         <v>490000.0</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>18</v>
+      <c r="D16" s="6">
+        <v>1901.67</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" s="4">
         <v>800000.0</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>18</v>
+      <c r="D17" s="6">
+        <v>2775.6</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C18" s="4">
         <v>450000.0</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>44</v>
+      <c r="D18" s="6">
+        <v>2143.62</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C19" s="4">
         <v>330000.0</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>44</v>
+      <c r="D19" s="6">
+        <v>4628.57</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" s="4">
         <v>220000.0</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>44</v>
+      <c r="D20" s="6">
+        <v>3515.25</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C21" s="4">
         <v>100000.0</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>51</v>
+      <c r="D21" s="5">
+        <v>141.05</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="4">
         <v>140000.0</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>51</v>
+      <c r="D22" s="5">
+        <v>150.46</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" s="4">
         <v>13000.0</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>51</v>
+      <c r="D23" s="5">
+        <v>29.6</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1"/>

</xml_diff>